<commit_message>
modified demos after day 3 of JDX course in London
</commit_message>
<xml_diff>
--- a/Python/src/Financial Python/Spreadsheets/data/empty.xlsx
+++ b/Python/src/Financial Python/Spreadsheets/data/empty.xlsx
@@ -6,9 +6,9 @@
     <s:workbookView activeTab="0"/>
   </s:bookViews>
   <s:sheets>
-    <s:sheet name="Sheet 0" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Sheet 1" sheetId="2" r:id="rId2"/>
-    <s:sheet name="Sheet 2" sheetId="3" r:id="rId3"/>
+    <s:sheet name="Sheet A" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Sheet B" sheetId="2" r:id="rId2"/>
+    <s:sheet name="Sheet C" sheetId="3" r:id="rId3"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>